<commit_message>
xlsx can handle google drive image link
</commit_message>
<xml_diff>
--- a/content/journals.xlsx
+++ b/content/journals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarut\Documents\Github\cept\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86C4364-8175-4410-976D-79AF7C3188A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F324A1-6534-4E4E-AC25-3F5F4D0EAE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,6 +335,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -388,7 +389,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -696,10 +697,13 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="53.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>